<commit_message>
Ajout du bilan mi-parcours. Code des tests en cours de modif
</commit_message>
<xml_diff>
--- a/Simulations/tests/resultats/donnees.xlsx
+++ b/Simulations/tests/resultats/donnees.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5880" yWindow="0" windowWidth="25600" windowHeight="14420" tabRatio="500"/>
+    <workbookView xWindow="10540" yWindow="0" windowWidth="13260" windowHeight="14420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TTFF_alea" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ttff" localSheetId="0">TTFF_alea!$A$3:$H$54</definedName>
+    <definedName name="ttff" localSheetId="0">TTFF_alea!$A$3:$H$49</definedName>
+    <definedName name="ttff_1" localSheetId="0">TTFF_alea!$A$2:$H$41</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,21 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="ttff.txt" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:Clo:Documents:Fac:M1:S2:TER:git:Simulations:tests:resultats:topologie_alea:ttff.txt" decimal="," thousands=" " tab="0" semicolon="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:Clo:Documents:Fac:M1:S2:TER:git:Simulations:tests:resultats:topologie_alea:ttff.txt" decimal="," thousands=" " tab="0" semicolon="1">
+      <textFields count="8">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="ttff.txt1" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:Clo:Documents:Fac:M1:S2:TER:git:Simulations:tests:resultats:topologie_alea:ttff.txt" decimal="," thousands=" " tab="0" semicolon="1">
       <textFields count="8">
         <textField/>
         <textField/>
@@ -41,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="7">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -68,13 +83,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
-  </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -97,14 +125,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="13">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -112,7 +164,641 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TTFF_alea!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FLOOD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>TTFF_alea!$I$2:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.4669585</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.499</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.525</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.579</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.631111</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.636</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.755556</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.826125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TTFF_alea!$J$2:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>126.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>126.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>126.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>126.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>126.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>126.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>126.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>126.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TTFF_alea!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RBOP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>TTFF_alea!$I$2:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.4669585</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.499</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.525</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.579</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.631111</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.636</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.755556</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.826125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TTFF_alea!$K$2:$K$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>118.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>118.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>117.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>118.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>118.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>118.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>118.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>118.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TTFF_alea!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LBOP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>TTFF_alea!$I$2:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.4669585</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.499</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.525</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.579</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.631111</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.636</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.755556</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.826125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TTFF_alea!$L$2:$L$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>115.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>116.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>116.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>116.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>116.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>116.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>116.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>116.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TTFF_alea!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BIP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>TTFF_alea!$I$2:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.4669585</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.499</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.525</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.579</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.631111</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.636</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.755556</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.826125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TTFF_alea!$M$2:$M$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>415.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>236.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>435.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>410.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>415.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>305.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>193.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>278.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TTFF_alea!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LBIP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>TTFF_alea!$I$2:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.4669585</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.499</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.525</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.579</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.631111</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.636</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.755556</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.826125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TTFF_alea!$N$2:$N$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>258.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>196.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>188.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>217.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>208.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>261.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>223.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>277.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TTFF_alea!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DLBIP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>TTFF_alea!$I$2:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.4669585</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.499</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.525</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.579</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.631111</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.636</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.755556</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.826125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TTFF_alea!$O$2:$O$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>247.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>196.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>177.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>226.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>176.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>223.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>235.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>247.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2082575448"/>
+        <c:axId val="2082576856"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2082575448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2082576856"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2082576856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2082575448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ttff_1" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ttff" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -438,144 +1124,330 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H54"/>
+  <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="I1" sqref="I1:O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="8" width="10.83203125" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="1" customWidth="1"/>
+    <col min="2" max="8" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8">
-      <c r="B2" t="s">
+    <row r="1" spans="1:15">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I1" s="1"/>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="1">
+        <v>0.46545500000000001</v>
+      </c>
+      <c r="B2">
+        <v>126</v>
+      </c>
+      <c r="C2">
+        <v>120</v>
+      </c>
+      <c r="D2">
+        <v>116</v>
+      </c>
+      <c r="E2">
+        <v>356</v>
+      </c>
+      <c r="F2">
+        <v>178</v>
+      </c>
+      <c r="G2">
+        <v>174</v>
+      </c>
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <f>AVERAGE(A2:A9)</f>
+        <v>0.46695850000000005</v>
+      </c>
+      <c r="J2" s="1">
+        <f t="shared" ref="J2:O2" si="0">AVERAGE(B2:B9)</f>
+        <v>126</v>
+      </c>
+      <c r="K2" s="1">
+        <f t="shared" si="0"/>
+        <v>118</v>
+      </c>
+      <c r="L2" s="1">
+        <f t="shared" si="0"/>
+        <v>115.75</v>
+      </c>
+      <c r="M2" s="1">
+        <f t="shared" si="0"/>
+        <v>415.25</v>
+      </c>
+      <c r="N2" s="1">
+        <f t="shared" si="0"/>
+        <v>258</v>
+      </c>
+      <c r="O2" s="1">
+        <f t="shared" si="0"/>
+        <v>247.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="1">
-        <v>0.56299999999999994</v>
+        <v>0.46545500000000001</v>
       </c>
       <c r="B3">
         <v>126</v>
       </c>
       <c r="C3">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D3">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E3">
-        <v>234</v>
+        <v>320</v>
       </c>
       <c r="F3">
+        <v>196</v>
+      </c>
+      <c r="G3">
         <v>206</v>
       </c>
-      <c r="G3">
-        <v>190</v>
-      </c>
       <c r="H3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" s="1">
+        <f>AVERAGE(A10:A13)</f>
+        <v>0.499</v>
+      </c>
+      <c r="J3" s="1">
+        <f t="shared" ref="J3:O3" si="1">AVERAGE(B10:B13)</f>
+        <v>126</v>
+      </c>
+      <c r="K3" s="1">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+      <c r="L3" s="1">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+      <c r="M3" s="1">
+        <f t="shared" si="1"/>
+        <v>236.5</v>
+      </c>
+      <c r="N3" s="1">
+        <f t="shared" si="1"/>
+        <v>196</v>
+      </c>
+      <c r="O3" s="1">
+        <f t="shared" si="1"/>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="1">
-        <v>0.41</v>
+        <v>0.46545500000000001</v>
       </c>
       <c r="B4">
         <v>126</v>
       </c>
       <c r="C4">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D4">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E4">
-        <v>496</v>
+        <v>292</v>
       </c>
       <c r="F4">
-        <v>160</v>
+        <v>174</v>
       </c>
       <c r="G4">
-        <v>148</v>
+        <v>180</v>
       </c>
       <c r="H4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4" s="1">
+        <f>AVERAGE(A14:A17)</f>
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" ref="J4:O4" si="2">AVERAGE(B14:B17)</f>
+        <v>126</v>
+      </c>
+      <c r="K4" s="1">
+        <f t="shared" si="2"/>
+        <v>117.5</v>
+      </c>
+      <c r="L4" s="1">
+        <f t="shared" si="2"/>
+        <v>116</v>
+      </c>
+      <c r="M4" s="1">
+        <f t="shared" si="2"/>
+        <v>435</v>
+      </c>
+      <c r="N4" s="1">
+        <f t="shared" si="2"/>
+        <v>188</v>
+      </c>
+      <c r="O4" s="1">
+        <f t="shared" si="2"/>
+        <v>177.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="1">
-        <v>0.62777799999999995</v>
+        <v>0.46545500000000001</v>
       </c>
       <c r="B5">
         <v>126</v>
       </c>
       <c r="C5">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D5">
         <v>114</v>
       </c>
       <c r="E5">
-        <v>450</v>
+        <v>268</v>
       </c>
       <c r="F5">
-        <v>226</v>
+        <v>164</v>
       </c>
       <c r="G5">
-        <v>228</v>
+        <v>172</v>
       </c>
       <c r="H5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" s="1">
+        <f>AVERAGE(A18:A21)</f>
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" ref="J5:O5" si="3">AVERAGE(B18:B21)</f>
+        <v>126</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="3"/>
+        <v>118.5</v>
+      </c>
+      <c r="L5" s="1">
+        <f t="shared" si="3"/>
+        <v>116</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="shared" si="3"/>
+        <v>410.5</v>
+      </c>
+      <c r="N5" s="1">
+        <f t="shared" si="3"/>
+        <v>217</v>
+      </c>
+      <c r="O5" s="1">
+        <f t="shared" si="3"/>
+        <v>226.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="1">
-        <v>0.511818</v>
+        <v>0.46846199999999999</v>
       </c>
       <c r="B6">
         <v>126</v>
       </c>
       <c r="C6">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D6">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E6">
-        <v>334</v>
+        <v>600</v>
       </c>
       <c r="F6">
-        <v>170</v>
+        <v>398</v>
       </c>
       <c r="G6">
-        <v>174</v>
+        <v>268</v>
       </c>
       <c r="H6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6" s="1">
+        <f>AVERAGE(A22:A25)</f>
+        <v>0.63111099999999998</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" ref="J6:O6" si="4">AVERAGE(B22:B25)</f>
+        <v>126</v>
+      </c>
+      <c r="K6" s="1">
+        <f t="shared" si="4"/>
+        <v>118</v>
+      </c>
+      <c r="L6" s="1">
+        <f t="shared" si="4"/>
+        <v>116</v>
+      </c>
+      <c r="M6" s="1">
+        <f t="shared" si="4"/>
+        <v>415</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" si="4"/>
+        <v>208.5</v>
+      </c>
+      <c r="O6" s="1">
+        <f t="shared" si="4"/>
+        <v>176.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="1">
-        <v>0.69444399999999995</v>
+        <v>0.46846199999999999</v>
       </c>
       <c r="B7">
         <v>126</v>
@@ -587,21 +1459,49 @@
         <v>118</v>
       </c>
       <c r="E7">
-        <v>374</v>
+        <v>484</v>
       </c>
       <c r="F7">
-        <v>264</v>
+        <v>286</v>
       </c>
       <c r="G7">
-        <v>224</v>
+        <v>314</v>
       </c>
       <c r="H7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7" s="1">
+        <f>AVERAGE(A26:A29)</f>
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" ref="J7:O7" si="5">AVERAGE(B26:B29)</f>
+        <v>126</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" si="5"/>
+        <v>118.5</v>
+      </c>
+      <c r="L7" s="1">
+        <f t="shared" si="5"/>
+        <v>116.5</v>
+      </c>
+      <c r="M7" s="1">
+        <f t="shared" si="5"/>
+        <v>305</v>
+      </c>
+      <c r="N7" s="1">
+        <f t="shared" si="5"/>
+        <v>261.5</v>
+      </c>
+      <c r="O7" s="1">
+        <f t="shared" si="5"/>
+        <v>223.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="1">
-        <v>0.52363599999999999</v>
+        <v>0.46846199999999999</v>
       </c>
       <c r="B8">
         <v>126</v>
@@ -613,21 +1513,49 @@
         <v>116</v>
       </c>
       <c r="E8">
-        <v>366</v>
+        <v>452</v>
       </c>
       <c r="F8">
-        <v>186</v>
+        <v>308</v>
       </c>
       <c r="G8">
-        <v>166</v>
+        <v>324</v>
       </c>
       <c r="H8" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8" s="1">
+        <f>AVERAGE(A30:A33)</f>
+        <v>0.75555600000000001</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" ref="J8:O8" si="6">AVERAGE(B30:B33)</f>
+        <v>126</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="6"/>
+        <v>118</v>
+      </c>
+      <c r="L8" s="1">
+        <f t="shared" si="6"/>
+        <v>116</v>
+      </c>
+      <c r="M8" s="1">
+        <f t="shared" si="6"/>
+        <v>193</v>
+      </c>
+      <c r="N8" s="1">
+        <f t="shared" si="6"/>
+        <v>223</v>
+      </c>
+      <c r="O8" s="1">
+        <f t="shared" si="6"/>
+        <v>235.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="1">
-        <v>0.64666699999999999</v>
+        <v>0.46846199999999999</v>
       </c>
       <c r="B9">
         <v>126</v>
@@ -636,24 +1564,52 @@
         <v>116</v>
       </c>
       <c r="D9">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E9">
-        <v>344</v>
+        <v>550</v>
       </c>
       <c r="F9">
-        <v>170</v>
+        <v>360</v>
       </c>
       <c r="G9">
-        <v>168</v>
+        <v>342</v>
       </c>
       <c r="H9" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9" s="1">
+        <f>AVERAGE(A34:A41)</f>
+        <v>0.826125</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" ref="J9:O9" si="7">AVERAGE(B34:B41)</f>
+        <v>126</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" si="7"/>
+        <v>118.25</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" si="7"/>
+        <v>116.5</v>
+      </c>
+      <c r="M9" s="1">
+        <f t="shared" si="7"/>
+        <v>278.25</v>
+      </c>
+      <c r="N9" s="1">
+        <f t="shared" si="7"/>
+        <v>277</v>
+      </c>
+      <c r="O9" s="1">
+        <f t="shared" si="7"/>
+        <v>247.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="1">
-        <v>0.45916699999999999</v>
+        <v>0.499</v>
       </c>
       <c r="B10">
         <v>126</v>
@@ -662,24 +1618,24 @@
         <v>118</v>
       </c>
       <c r="D10">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E10">
-        <v>350</v>
+        <v>210</v>
       </c>
       <c r="F10">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="G10">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="H10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:15">
       <c r="A11" s="1">
-        <v>0.42454500000000001</v>
+        <v>0.499</v>
       </c>
       <c r="B11">
         <v>126</v>
@@ -688,24 +1644,24 @@
         <v>120</v>
       </c>
       <c r="D11">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E11">
-        <v>426</v>
+        <v>226</v>
       </c>
       <c r="F11">
-        <v>272</v>
+        <v>186</v>
       </c>
       <c r="G11">
-        <v>326</v>
+        <v>172</v>
       </c>
       <c r="H11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:15">
       <c r="A12" s="1">
-        <v>0.68899999999999995</v>
+        <v>0.499</v>
       </c>
       <c r="B12">
         <v>126</v>
@@ -714,102 +1670,102 @@
         <v>118</v>
       </c>
       <c r="D12">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E12">
-        <v>378</v>
+        <v>258</v>
       </c>
       <c r="F12">
+        <v>194</v>
+      </c>
+      <c r="G12">
+        <v>214</v>
+      </c>
+      <c r="H12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="1">
+        <v>0.499</v>
+      </c>
+      <c r="B13">
+        <v>126</v>
+      </c>
+      <c r="C13">
+        <v>116</v>
+      </c>
+      <c r="D13">
+        <v>114</v>
+      </c>
+      <c r="E13">
+        <v>252</v>
+      </c>
+      <c r="F13">
+        <v>200</v>
+      </c>
+      <c r="G13">
+        <v>196</v>
+      </c>
+      <c r="H13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="1">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="B14">
+        <v>126</v>
+      </c>
+      <c r="C14">
+        <v>116</v>
+      </c>
+      <c r="D14">
+        <v>116</v>
+      </c>
+      <c r="E14">
+        <v>502</v>
+      </c>
+      <c r="F14">
+        <v>182</v>
+      </c>
+      <c r="G14">
+        <v>180</v>
+      </c>
+      <c r="H14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="1">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="B15">
+        <v>126</v>
+      </c>
+      <c r="C15">
+        <v>120</v>
+      </c>
+      <c r="D15">
+        <v>118</v>
+      </c>
+      <c r="E15">
+        <v>414</v>
+      </c>
+      <c r="F15">
+        <v>190</v>
+      </c>
+      <c r="G15">
         <v>186</v>
       </c>
-      <c r="G12">
-        <v>194</v>
-      </c>
-      <c r="H12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="1">
-        <v>0.48199999999999998</v>
-      </c>
-      <c r="B13">
-        <v>126</v>
-      </c>
-      <c r="C13">
-        <v>118</v>
-      </c>
-      <c r="D13">
-        <v>116</v>
-      </c>
-      <c r="E13">
-        <v>402</v>
-      </c>
-      <c r="F13">
-        <v>138</v>
-      </c>
-      <c r="G13">
-        <v>158</v>
-      </c>
-      <c r="H13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="1">
-        <v>0.72875000000000001</v>
-      </c>
-      <c r="B14">
-        <v>126</v>
-      </c>
-      <c r="C14">
-        <v>118</v>
-      </c>
-      <c r="D14">
-        <v>116</v>
-      </c>
-      <c r="E14">
-        <v>330</v>
-      </c>
-      <c r="F14">
-        <v>152</v>
-      </c>
-      <c r="G14">
-        <v>198</v>
-      </c>
-      <c r="H14" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="1">
-        <v>0.67888899999999996</v>
-      </c>
-      <c r="B15">
-        <v>126</v>
-      </c>
-      <c r="C15">
-        <v>118</v>
-      </c>
-      <c r="D15">
-        <v>118</v>
-      </c>
-      <c r="E15">
-        <v>302</v>
-      </c>
-      <c r="F15">
-        <v>240</v>
-      </c>
-      <c r="G15">
-        <v>254</v>
-      </c>
       <c r="H15" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:15">
       <c r="A16" s="1">
-        <v>0.661111</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="B16">
         <v>126</v>
@@ -818,13 +1774,13 @@
         <v>118</v>
       </c>
       <c r="D16">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E16">
-        <v>276</v>
+        <v>432</v>
       </c>
       <c r="F16">
-        <v>144</v>
+        <v>190</v>
       </c>
       <c r="G16">
         <v>164</v>
@@ -835,7 +1791,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1">
-        <v>0.410769</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="B17">
         <v>126</v>
@@ -844,16 +1800,16 @@
         <v>116</v>
       </c>
       <c r="D17">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E17">
-        <v>482</v>
+        <v>392</v>
       </c>
       <c r="F17">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="G17">
-        <v>208</v>
+        <v>180</v>
       </c>
       <c r="H17" t="s">
         <v>0</v>
@@ -861,25 +1817,25 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1">
-        <v>0.516154</v>
+        <v>0.57899999999999996</v>
       </c>
       <c r="B18">
         <v>126</v>
       </c>
       <c r="C18">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D18">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E18">
-        <v>336</v>
+        <v>424</v>
       </c>
       <c r="F18">
-        <v>362</v>
+        <v>204</v>
       </c>
       <c r="G18">
-        <v>252</v>
+        <v>270</v>
       </c>
       <c r="H18" t="s">
         <v>0</v>
@@ -887,7 +1843,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1">
-        <v>0.378</v>
+        <v>0.57899999999999996</v>
       </c>
       <c r="B19">
         <v>126</v>
@@ -896,16 +1852,16 @@
         <v>120</v>
       </c>
       <c r="D19">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E19">
-        <v>320</v>
+        <v>412</v>
       </c>
       <c r="F19">
-        <v>244</v>
+        <v>220</v>
       </c>
       <c r="G19">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="H19" t="s">
         <v>0</v>
@@ -913,7 +1869,7 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1">
-        <v>0.39833299999999999</v>
+        <v>0.57899999999999996</v>
       </c>
       <c r="B20">
         <v>126</v>
@@ -925,13 +1881,13 @@
         <v>116</v>
       </c>
       <c r="E20">
-        <v>250</v>
+        <v>370</v>
       </c>
       <c r="F20">
-        <v>188</v>
+        <v>230</v>
       </c>
       <c r="G20">
-        <v>198</v>
+        <v>230</v>
       </c>
       <c r="H20" t="s">
         <v>0</v>
@@ -939,7 +1895,7 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1">
-        <v>0.77777799999999997</v>
+        <v>0.57899999999999996</v>
       </c>
       <c r="B21">
         <v>126</v>
@@ -948,16 +1904,16 @@
         <v>116</v>
       </c>
       <c r="D21">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E21">
-        <v>298</v>
+        <v>436</v>
       </c>
       <c r="F21">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="G21">
-        <v>208</v>
+        <v>186</v>
       </c>
       <c r="H21" t="s">
         <v>0</v>
@@ -965,25 +1921,25 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1">
-        <v>0.55500000000000005</v>
+        <v>0.63111099999999998</v>
       </c>
       <c r="B22">
         <v>126</v>
       </c>
       <c r="C22">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D22">
         <v>116</v>
       </c>
       <c r="E22">
-        <v>476</v>
+        <v>376</v>
       </c>
       <c r="F22">
-        <v>226</v>
+        <v>202</v>
       </c>
       <c r="G22">
-        <v>212</v>
+        <v>174</v>
       </c>
       <c r="H22" t="s">
         <v>0</v>
@@ -991,25 +1947,25 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1">
-        <v>0.47090900000000002</v>
+        <v>0.63111099999999998</v>
       </c>
       <c r="B23">
         <v>126</v>
       </c>
       <c r="C23">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D23">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E23">
-        <v>300</v>
+        <v>432</v>
       </c>
       <c r="F23">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="G23">
-        <v>208</v>
+        <v>186</v>
       </c>
       <c r="H23" t="s">
         <v>0</v>
@@ -1017,7 +1973,7 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1">
-        <v>0.807778</v>
+        <v>0.63111099999999998</v>
       </c>
       <c r="B24">
         <v>126</v>
@@ -1026,16 +1982,16 @@
         <v>118</v>
       </c>
       <c r="D24">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E24">
-        <v>286</v>
+        <v>396</v>
       </c>
       <c r="F24">
-        <v>234</v>
+        <v>198</v>
       </c>
       <c r="G24">
-        <v>222</v>
+        <v>166</v>
       </c>
       <c r="H24" t="s">
         <v>0</v>
@@ -1043,25 +1999,25 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1">
-        <v>0.39916699999999999</v>
+        <v>0.63111099999999998</v>
       </c>
       <c r="B25">
         <v>126</v>
       </c>
       <c r="C25">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D25">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E25">
-        <v>402</v>
+        <v>456</v>
       </c>
       <c r="F25">
-        <v>192</v>
+        <v>212</v>
       </c>
       <c r="G25">
-        <v>154</v>
+        <v>180</v>
       </c>
       <c r="H25" t="s">
         <v>0</v>
@@ -1069,25 +2025,25 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1">
-        <v>0.58799999999999997</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="B26">
         <v>126</v>
       </c>
       <c r="C26">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D26">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E26">
-        <v>236</v>
+        <v>304</v>
       </c>
       <c r="F26">
-        <v>196</v>
+        <v>266</v>
       </c>
       <c r="G26">
-        <v>196</v>
+        <v>220</v>
       </c>
       <c r="H26" t="s">
         <v>0</v>
@@ -1095,25 +2051,25 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1">
-        <v>0.51600000000000001</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="B27">
         <v>126</v>
       </c>
       <c r="C27">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D27">
         <v>118</v>
       </c>
       <c r="E27">
-        <v>344</v>
+        <v>290</v>
       </c>
       <c r="F27">
-        <v>212</v>
+        <v>274</v>
       </c>
       <c r="G27">
-        <v>200</v>
+        <v>242</v>
       </c>
       <c r="H27" t="s">
         <v>0</v>
@@ -1121,7 +2077,7 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1">
-        <v>0.56899999999999995</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="B28">
         <v>126</v>
@@ -1133,13 +2089,13 @@
         <v>116</v>
       </c>
       <c r="E28">
-        <v>252</v>
+        <v>292</v>
       </c>
       <c r="F28">
-        <v>172</v>
+        <v>238</v>
       </c>
       <c r="G28">
-        <v>188</v>
+        <v>226</v>
       </c>
       <c r="H28" t="s">
         <v>0</v>
@@ -1147,25 +2103,25 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1">
-        <v>0.54700000000000004</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="B29">
         <v>126</v>
       </c>
       <c r="C29">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D29">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E29">
-        <v>318</v>
+        <v>334</v>
       </c>
       <c r="F29">
-        <v>162</v>
+        <v>268</v>
       </c>
       <c r="G29">
-        <v>142</v>
+        <v>206</v>
       </c>
       <c r="H29" t="s">
         <v>0</v>
@@ -1173,7 +2129,7 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1">
-        <v>0.44083299999999997</v>
+        <v>0.75555600000000001</v>
       </c>
       <c r="B30">
         <v>126</v>
@@ -1185,13 +2141,13 @@
         <v>116</v>
       </c>
       <c r="E30">
-        <v>344</v>
+        <v>210</v>
       </c>
       <c r="F30">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="G30">
-        <v>180</v>
+        <v>238</v>
       </c>
       <c r="H30" t="s">
         <v>0</v>
@@ -1199,7 +2155,7 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1">
-        <v>0.50166699999999997</v>
+        <v>0.75555600000000001</v>
       </c>
       <c r="B31">
         <v>126</v>
@@ -1208,16 +2164,16 @@
         <v>120</v>
       </c>
       <c r="D31">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E31">
-        <v>262</v>
+        <v>220</v>
       </c>
       <c r="F31">
-        <v>202</v>
+        <v>236</v>
       </c>
       <c r="G31">
-        <v>256</v>
+        <v>220</v>
       </c>
       <c r="H31" t="s">
         <v>0</v>
@@ -1225,7 +2181,7 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1">
-        <v>0.626</v>
+        <v>0.75555600000000001</v>
       </c>
       <c r="B32">
         <v>126</v>
@@ -1237,13 +2193,13 @@
         <v>116</v>
       </c>
       <c r="E32">
-        <v>266</v>
+        <v>176</v>
       </c>
       <c r="F32">
-        <v>206</v>
+        <v>240</v>
       </c>
       <c r="G32">
-        <v>198</v>
+        <v>254</v>
       </c>
       <c r="H32" t="s">
         <v>0</v>
@@ -1251,25 +2207,25 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1">
-        <v>0.41636400000000001</v>
+        <v>0.75555600000000001</v>
       </c>
       <c r="B33">
         <v>126</v>
       </c>
       <c r="C33">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D33">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E33">
-        <v>398</v>
+        <v>166</v>
       </c>
       <c r="F33">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="G33">
-        <v>190</v>
+        <v>230</v>
       </c>
       <c r="H33" t="s">
         <v>0</v>
@@ -1277,7 +2233,7 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1">
-        <v>0.78500000000000003</v>
+        <v>0.82599999999999996</v>
       </c>
       <c r="B34">
         <v>126</v>
@@ -1286,16 +2242,16 @@
         <v>118</v>
       </c>
       <c r="D34">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E34">
-        <v>300</v>
+        <v>342</v>
       </c>
       <c r="F34">
-        <v>260</v>
+        <v>342</v>
       </c>
       <c r="G34">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="H34" t="s">
         <v>0</v>
@@ -1303,25 +2259,25 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1">
-        <v>0.73888900000000002</v>
+        <v>0.82599999999999996</v>
       </c>
       <c r="B35">
         <v>126</v>
       </c>
       <c r="C35">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D35">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E35">
-        <v>254</v>
+        <v>292</v>
       </c>
       <c r="F35">
-        <v>264</v>
+        <v>348</v>
       </c>
       <c r="G35">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="H35" t="s">
         <v>0</v>
@@ -1329,25 +2285,25 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1">
-        <v>0.42833300000000002</v>
+        <v>0.82599999999999996</v>
       </c>
       <c r="B36">
         <v>126</v>
       </c>
       <c r="C36">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D36">
         <v>116</v>
       </c>
       <c r="E36">
-        <v>244</v>
+        <v>290</v>
       </c>
       <c r="F36">
-        <v>236</v>
+        <v>272</v>
       </c>
       <c r="G36">
-        <v>236</v>
+        <v>260</v>
       </c>
       <c r="H36" t="s">
         <v>0</v>
@@ -1355,25 +2311,25 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1">
-        <v>0.44333299999999998</v>
+        <v>0.82599999999999996</v>
       </c>
       <c r="B37">
         <v>126</v>
       </c>
       <c r="C37">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D37">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E37">
-        <v>252</v>
+        <v>288</v>
       </c>
       <c r="F37">
-        <v>226</v>
+        <v>334</v>
       </c>
       <c r="G37">
-        <v>168</v>
+        <v>276</v>
       </c>
       <c r="H37" t="s">
         <v>0</v>
@@ -1381,7 +2337,7 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1">
-        <v>0.65300000000000002</v>
+        <v>0.82625000000000004</v>
       </c>
       <c r="B38">
         <v>126</v>
@@ -1390,16 +2346,16 @@
         <v>120</v>
       </c>
       <c r="D38">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="E38">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="F38">
-        <v>180</v>
+        <v>230</v>
       </c>
       <c r="G38">
-        <v>196</v>
+        <v>268</v>
       </c>
       <c r="H38" t="s">
         <v>0</v>
@@ -1407,25 +2363,25 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1">
-        <v>0.46333299999999999</v>
+        <v>0.82625000000000004</v>
       </c>
       <c r="B39">
         <v>126</v>
       </c>
       <c r="C39">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D39">
         <v>118</v>
       </c>
       <c r="E39">
-        <v>400</v>
+        <v>274</v>
       </c>
       <c r="F39">
-        <v>348</v>
+        <v>200</v>
       </c>
       <c r="G39">
-        <v>236</v>
+        <v>204</v>
       </c>
       <c r="H39" t="s">
         <v>0</v>
@@ -1433,25 +2389,25 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1">
-        <v>0.53454500000000005</v>
+        <v>0.82625000000000004</v>
       </c>
       <c r="B40">
         <v>126</v>
       </c>
       <c r="C40">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D40">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E40">
-        <v>466</v>
+        <v>246</v>
       </c>
       <c r="F40">
-        <v>256</v>
+        <v>218</v>
       </c>
       <c r="G40">
-        <v>214</v>
+        <v>250</v>
       </c>
       <c r="H40" t="s">
         <v>0</v>
@@ -1459,370 +2415,37 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1">
-        <v>0.67333299999999996</v>
+        <v>0.82625000000000004</v>
       </c>
       <c r="B41">
         <v>126</v>
       </c>
       <c r="C41">
+        <v>116</v>
+      </c>
+      <c r="D41">
         <v>114</v>
       </c>
-      <c r="D41">
-        <v>116</v>
-      </c>
       <c r="E41">
-        <v>390</v>
+        <v>258</v>
       </c>
       <c r="F41">
-        <v>194</v>
+        <v>272</v>
       </c>
       <c r="G41">
-        <v>174</v>
+        <v>228</v>
       </c>
       <c r="H41" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="1">
-        <v>0.50600000000000001</v>
-      </c>
-      <c r="B42">
-        <v>126</v>
-      </c>
-      <c r="C42">
-        <v>120</v>
-      </c>
-      <c r="D42">
-        <v>116</v>
-      </c>
-      <c r="E42">
-        <v>362</v>
-      </c>
-      <c r="F42">
-        <v>156</v>
-      </c>
-      <c r="G42">
-        <v>160</v>
-      </c>
-      <c r="H42" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="1">
-        <v>0.32153799999999999</v>
-      </c>
-      <c r="B43">
-        <v>126</v>
-      </c>
-      <c r="C43">
-        <v>118</v>
-      </c>
-      <c r="D43">
-        <v>116</v>
-      </c>
-      <c r="E43">
-        <v>312</v>
-      </c>
-      <c r="F43">
-        <v>182</v>
-      </c>
-      <c r="G43">
-        <v>192</v>
-      </c>
-      <c r="H43" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="1">
-        <v>0.82250000000000001</v>
-      </c>
-      <c r="B44">
-        <v>126</v>
-      </c>
-      <c r="C44">
-        <v>120</v>
-      </c>
-      <c r="D44">
-        <v>118</v>
-      </c>
-      <c r="E44">
-        <v>272</v>
-      </c>
-      <c r="F44">
-        <v>176</v>
-      </c>
-      <c r="G44">
-        <v>188</v>
-      </c>
-      <c r="H44" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="1">
-        <v>0.37</v>
-      </c>
-      <c r="B45">
-        <v>126</v>
-      </c>
-      <c r="C45">
-        <v>118</v>
-      </c>
-      <c r="D45">
-        <v>114</v>
-      </c>
-      <c r="E45">
-        <v>392</v>
-      </c>
-      <c r="F45">
-        <v>216</v>
-      </c>
-      <c r="G45">
-        <v>232</v>
-      </c>
-      <c r="H45" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="1">
-        <v>0.39833299999999999</v>
-      </c>
-      <c r="B46">
-        <v>126</v>
-      </c>
-      <c r="C46">
-        <v>120</v>
-      </c>
-      <c r="D46">
-        <v>116</v>
-      </c>
-      <c r="E46">
-        <v>320</v>
-      </c>
-      <c r="F46">
-        <v>240</v>
-      </c>
-      <c r="G46">
-        <v>338</v>
-      </c>
-      <c r="H46" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="1">
-        <v>0.408333</v>
-      </c>
-      <c r="B47">
-        <v>126</v>
-      </c>
-      <c r="C47">
-        <v>118</v>
-      </c>
-      <c r="D47">
-        <v>116</v>
-      </c>
-      <c r="E47">
-        <v>294</v>
-      </c>
-      <c r="F47">
-        <v>168</v>
-      </c>
-      <c r="G47">
-        <v>174</v>
-      </c>
-      <c r="H47" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="1">
-        <v>0.57222200000000001</v>
-      </c>
-      <c r="B48">
-        <v>126</v>
-      </c>
-      <c r="C48">
-        <v>120</v>
-      </c>
-      <c r="D48">
-        <v>116</v>
-      </c>
-      <c r="E48">
-        <v>378</v>
-      </c>
-      <c r="F48">
-        <v>214</v>
-      </c>
-      <c r="G48">
-        <v>214</v>
-      </c>
-      <c r="H48" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="1">
-        <v>0.72</v>
-      </c>
-      <c r="B49">
-        <v>126</v>
-      </c>
-      <c r="C49">
-        <v>118</v>
-      </c>
-      <c r="D49">
-        <v>116</v>
-      </c>
-      <c r="E49">
-        <v>206</v>
-      </c>
-      <c r="F49">
-        <v>280</v>
-      </c>
-      <c r="G49">
-        <v>344</v>
-      </c>
-      <c r="H49" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
-      <c r="A50" s="1">
-        <v>0.46</v>
-      </c>
-      <c r="B50">
-        <v>126</v>
-      </c>
-      <c r="C50">
-        <v>118</v>
-      </c>
-      <c r="D50">
-        <v>118</v>
-      </c>
-      <c r="E50">
-        <v>294</v>
-      </c>
-      <c r="F50">
-        <v>220</v>
-      </c>
-      <c r="G50">
-        <v>194</v>
-      </c>
-      <c r="H50" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" s="1">
-        <v>0.48199999999999998</v>
-      </c>
-      <c r="B51">
-        <v>126</v>
-      </c>
-      <c r="C51">
-        <v>120</v>
-      </c>
-      <c r="D51">
-        <v>116</v>
-      </c>
-      <c r="E51">
-        <v>228</v>
-      </c>
-      <c r="F51">
-        <v>218</v>
-      </c>
-      <c r="G51">
-        <v>198</v>
-      </c>
-      <c r="H51" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="1">
-        <v>0.72</v>
-      </c>
-      <c r="B52">
-        <v>126</v>
-      </c>
-      <c r="C52">
-        <v>120</v>
-      </c>
-      <c r="D52">
-        <v>116</v>
-      </c>
-      <c r="E52">
-        <v>334</v>
-      </c>
-      <c r="F52">
-        <v>222</v>
-      </c>
-      <c r="G52">
-        <v>204</v>
-      </c>
-      <c r="H52" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
-      <c r="A53" s="1">
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="B53">
-        <v>126</v>
-      </c>
-      <c r="C53">
-        <v>118</v>
-      </c>
-      <c r="D53">
-        <v>116</v>
-      </c>
-      <c r="E53">
-        <v>468</v>
-      </c>
-      <c r="F53">
-        <v>180</v>
-      </c>
-      <c r="G53">
-        <v>176</v>
-      </c>
-      <c r="H53" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="A54" s="1">
-        <v>0.51600000000000001</v>
-      </c>
-      <c r="B54">
-        <v>126</v>
-      </c>
-      <c r="C54">
-        <v>120</v>
-      </c>
-      <c r="D54">
-        <v>116</v>
-      </c>
-      <c r="E54">
-        <v>426</v>
-      </c>
-      <c r="F54">
-        <v>292</v>
-      </c>
-      <c r="G54">
-        <v>252</v>
-      </c>
-      <c r="H54" t="s">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState ref="A2:G41">
+    <sortCondition ref="A2:A41"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>